<commit_message>
data atual no relatorio
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Criado</t>
   </si>
@@ -58,6 +58,72 @@
     <t>Obs</t>
   </si>
   <si>
+    <t>Mon Jun 28 2021 06:54:51 GMT-0300 (Horário Padrão de Brasília)</t>
+  </si>
+  <si>
+    <t>EQUIPE 3</t>
+  </si>
+  <si>
+    <t>OPERACIONAL 8</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>111.111.111-11</t>
+  </si>
+  <si>
+    <t>SAQUE COMPLEMENTAR</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>22,22</t>
+  </si>
+  <si>
+    <t>AGUARDANDO AVERB INSS</t>
+  </si>
+  <si>
+    <t>Mon Jun 28 2021 06:54:14 GMT-0300 (Horário Padrão de Brasília)</t>
+  </si>
+  <si>
+    <t>FGTS</t>
+  </si>
+  <si>
+    <t>Mon Jun 28 2021 06:53:44 GMT-0300 (Horário Padrão de Brasília)</t>
+  </si>
+  <si>
+    <t>CARTÃO</t>
+  </si>
+  <si>
+    <t>Mon Jun 28 2021 06:46:23 GMT-0300 (Horário Padrão de Brasília)</t>
+  </si>
+  <si>
+    <t>BRUNO FERNANDO GOMES DA SILVA</t>
+  </si>
+  <si>
+    <t>CREDITO CONTA</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Mon Jun 28 2021 06:45:49 GMT-0300 (Horário Padrão de Brasília)</t>
+  </si>
+  <si>
+    <t>EQUIPE 6</t>
+  </si>
+  <si>
+    <t>OPERACIONAL 6</t>
+  </si>
+  <si>
+    <t>PENDENTE</t>
+  </si>
+  <si>
     <t>Sun Jun 27 2021 00:30:17 GMT-0300 (Horário Padrão de Brasília)</t>
   </si>
   <si>
@@ -65,12 +131,6 @@
   </si>
   <si>
     <t>OPERACIONAL 7</t>
-  </si>
-  <si>
-    <t>BRUNO FERNANDO GOMES DA SILVA</t>
-  </si>
-  <si>
-    <t>111.111.111-11</t>
   </si>
   <si>
     <t>PORTABILIDADE</t>
@@ -98,9 +158,6 @@
     <t>Sun Jun 27 2021 00:07:11 GMT-0300 (Horário Padrão de Brasília)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>REFIN</t>
   </si>
   <si>
@@ -171,36 +228,6 @@
   </si>
   <si>
     <t>Fri Jun 25 2021 13:17:50 GMT-0300 (Horário Padrão de Brasília)</t>
-  </si>
-  <si>
-    <t>Mon Jun 28 2021 06:46:23 GMT-0300 (Horário Padrão de Brasília)</t>
-  </si>
-  <si>
-    <t>CREDITO CONTA</t>
-  </si>
-  <si>
-    <t>22,22</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>Observação</t>
-  </si>
-  <si>
-    <t>Mon Jun 28 2021 06:45:49 GMT-0300 (Horário Padrão de Brasília)</t>
-  </si>
-  <si>
-    <t>EQUIPE 6</t>
-  </si>
-  <si>
-    <t>OPERACIONAL 6</t>
-  </si>
-  <si>
-    <t>SAQUE COMPLEMENTAR</t>
-  </si>
-  <si>
-    <t>PENDENTE</t>
   </si>
 </sst>
 </file>
@@ -240,7 +267,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -295,13 +322,13 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>18</v>
@@ -310,45 +337,45 @@
         <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>18</v>
@@ -357,39 +384,39 @@
         <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -404,48 +431,48 @@
         <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="N4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>19</v>
@@ -454,45 +481,45 @@
         <v>5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>19</v>
@@ -507,39 +534,39 @@
         <v>7</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>19</v>
@@ -548,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>7</v>
@@ -560,33 +587,33 @@
         <v>9</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>19</v>
@@ -595,7 +622,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>7</v>
@@ -607,113 +634,348 @@
         <v>9</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>28</v>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>